<commit_message>
update symptoms check - michael
</commit_message>
<xml_diff>
--- a/forms/app/symptoms_check.xlsx
+++ b/forms/app/symptoms_check.xlsx
@@ -1,30 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/senseibara/Documents/MEDIC/config-cht-demo/forms/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelkohn/github/config-covid/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58498094-C8C0-824D-BFF3-755EB0E4970B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4160FCB4-2BB5-244A-A6D6-1617154C5215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6100" yWindow="1340" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="106">
   <si>
     <t>type</t>
   </si>
@@ -187,6 +185,12 @@
     <t>Phone No</t>
   </si>
   <si>
+    <t>patient_zero</t>
+  </si>
+  <si>
+    <t>Patient Zero UUID</t>
+  </si>
+  <si>
     <t>calculate</t>
   </si>
   <si>
@@ -208,6 +212,27 @@
     <t>../inputs/contact/_id</t>
   </si>
   <si>
+    <t>contact_info</t>
+  </si>
+  <si>
+    <t>Contact information</t>
+  </si>
+  <si>
+    <t>contact_patient_zero</t>
+  </si>
+  <si>
+    <t>Patient Zero</t>
+  </si>
+  <si>
+    <t>db-object bind-id-only</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>../../inputs/contact/patient_zero</t>
+  </si>
+  <si>
     <t>symptom_check</t>
   </si>
   <si>
@@ -218,9 +243,6 @@
   </si>
   <si>
     <t>result</t>
-  </si>
-  <si>
-    <t>Have you called the patient to check his symptoms report ?</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -230,9 +252,6 @@
     <t>symptom</t>
   </si>
   <si>
-    <t>Does the patient have any covid symptom</t>
-  </si>
-  <si>
     <t>Le patient présente-t-il des symptômes de convoitise?</t>
   </si>
   <si>
@@ -251,9 +270,18 @@
     <t>note</t>
   </si>
   <si>
+    <t>r_submit_note</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="text-align:center;"&gt;Click the Submit button at the bottom of the form.&lt;/h4&gt;</t>
+  </si>
+  <si>
     <t>r_summary_details</t>
   </si>
   <si>
+    <t>(Please note you can only report one signal at a time)</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -305,16 +333,25 @@
     <t>data</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h2 style="text-align:center;margin-bottom:0px;"&gt; Inform the care team to take over ${surname}&lt;/h2&gt; </t>
-  </si>
-  <si>
-    <t>tel</t>
-  </si>
-  <si>
-    <t>covid_patient</t>
-  </si>
-  <si>
-    <t>Patient with covid-19 UUID</t>
+    <t>Have you called the patient?</t>
+  </si>
+  <si>
+    <t>Is the ${other_names} experiencing COVID-19 symptoms?</t>
+  </si>
+  <si>
+    <t>Symptom Confirmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2 style="text-align:center;margin-bottom:0px;"&gt; Please refer ${other_names} to the Care Team&lt;/h2&gt; </t>
+  </si>
+  <si>
+    <t>r_refer</t>
+  </si>
+  <si>
+    <t>Referrals&lt;I class="fa fa-hospital-o"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h1 red</t>
   </si>
 </sst>
 </file>
@@ -461,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -518,6 +555,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -649,7 +694,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -945,20 +990,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP1048572"/>
+  <dimension ref="A1:AP1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
     <col min="4" max="4" width="56.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="7" width="24.83203125" customWidth="1"/>
@@ -1427,7 +1472,7 @@
     </row>
     <row r="9" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>40</v>
@@ -1479,7 +1524,7 @@
     </row>
     <row r="10" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>42</v>
@@ -1531,7 +1576,7 @@
     </row>
     <row r="11" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>44</v>
@@ -1583,7 +1628,7 @@
     </row>
     <row r="12" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>46</v>
@@ -1635,7 +1680,7 @@
     </row>
     <row r="13" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>48</v>
@@ -1687,16 +1732,16 @@
     </row>
     <row r="14" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1831,25 +1876,25 @@
     </row>
     <row r="17" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -1860,7 +1905,7 @@
       <c r="N17" s="18"/>
       <c r="O17" s="19"/>
       <c r="P17" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="17"/>
@@ -1888,18 +1933,18 @@
       <c r="AO17" s="17"/>
       <c r="AP17" s="17"/>
     </row>
-    <row r="18" spans="1:42" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
@@ -1907,153 +1952,170 @@
       <c r="H18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="23"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="21"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="23"/>
-      <c r="AG18" s="23"/>
-      <c r="AH18" s="23"/>
-      <c r="AI18" s="23"/>
-      <c r="AJ18" s="23"/>
-      <c r="AK18" s="23"/>
-      <c r="AL18" s="23"/>
-      <c r="AM18" s="23"/>
-      <c r="AN18" s="23"/>
-      <c r="AO18" s="23"/>
-      <c r="AP18" s="23"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="17"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="17"/>
+      <c r="AI18" s="17"/>
+      <c r="AJ18" s="17"/>
+      <c r="AK18" s="17"/>
+      <c r="AL18" s="17"/>
+      <c r="AM18" s="17"/>
+      <c r="AN18" s="17"/>
+      <c r="AO18" s="17"/>
+      <c r="AP18" s="17"/>
     </row>
-    <row r="19" spans="1:42" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>59</v>
+    <row r="19" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="C19" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>62</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="H19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="J19" s="21"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="23"/>
-      <c r="AG19" s="23"/>
-      <c r="AH19" s="23"/>
-      <c r="AI19" s="23"/>
-      <c r="AJ19" s="23"/>
-      <c r="AK19" s="23"/>
-      <c r="AL19" s="23"/>
-      <c r="AM19" s="23"/>
-      <c r="AN19" s="23"/>
-      <c r="AO19" s="23"/>
-      <c r="AP19" s="23"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="17"/>
+      <c r="AH19" s="17"/>
+      <c r="AI19" s="17"/>
+      <c r="AJ19" s="17"/>
+      <c r="AK19" s="17"/>
+      <c r="AL19" s="17"/>
+      <c r="AM19" s="17"/>
+      <c r="AN19" s="17"/>
+      <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
     </row>
-    <row r="20" spans="1:42" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27" t="s">
+    <row r="20" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="17"/>
+      <c r="AJ20" s="17"/>
+      <c r="AK20" s="17"/>
+      <c r="AL20" s="17"/>
+      <c r="AM20" s="17"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+    </row>
+    <row r="21" spans="1:42" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="27"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="27"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AD20" s="27"/>
-      <c r="AE20" s="27"/>
-    </row>
-    <row r="21" spans="1:42" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="C21" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
+      <c r="N21" s="28"/>
       <c r="O21" s="27"/>
       <c r="P21" s="27"/>
       <c r="Q21" s="27"/>
@@ -2071,112 +2133,359 @@
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
       <c r="AE21" s="27"/>
+      <c r="AF21" s="27"/>
+      <c r="AG21" s="27"/>
+      <c r="AH21" s="27"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="27"/>
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="27"/>
+      <c r="AO21" s="27"/>
+      <c r="AP21" s="27"/>
     </row>
-    <row r="22" spans="1:42" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="28" t="s">
+    <row r="22" spans="1:42" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="B22" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="27"/>
+      <c r="AE22" s="27"/>
+      <c r="AF22" s="27"/>
+      <c r="AG22" s="27"/>
+      <c r="AH22" s="27"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="27"/>
+      <c r="AK22" s="27"/>
+      <c r="AL22" s="27"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
+      <c r="AO22" s="27"/>
+      <c r="AP22" s="27"/>
+    </row>
+    <row r="23" spans="1:42" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="28"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="28"/>
-      <c r="AP22" s="28"/>
+      <c r="B23" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="31"/>
+      <c r="AE23" s="31"/>
     </row>
-    <row r="23" spans="1:42" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="32"/>
-      <c r="AE24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31"/>
     </row>
-    <row r="25" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:42" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="32"/>
+      <c r="AB25" s="32"/>
+      <c r="AC25" s="32"/>
+      <c r="AD25" s="32"/>
+      <c r="AE25" s="32"/>
+      <c r="AF25" s="32"/>
+      <c r="AG25" s="32"/>
+      <c r="AH25" s="32"/>
+      <c r="AI25" s="32"/>
+      <c r="AJ25" s="32"/>
+      <c r="AK25" s="32"/>
+      <c r="AL25" s="32"/>
+      <c r="AM25" s="32"/>
+      <c r="AN25" s="32"/>
+      <c r="AO25" s="32"/>
+      <c r="AP25" s="32"/>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="32"/>
+      <c r="AA26" s="32"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="32"/>
+      <c r="AD26" s="32"/>
+      <c r="AE26" s="32"/>
+      <c r="AF26" s="32"/>
+      <c r="AG26" s="32"/>
+      <c r="AH26" s="32"/>
+      <c r="AI26" s="32"/>
+      <c r="AJ26" s="32"/>
+      <c r="AK26" s="32"/>
+      <c r="AL26" s="32"/>
+      <c r="AM26" s="32"/>
+      <c r="AN26" s="32"/>
+      <c r="AO26" s="32"/>
+      <c r="AP26" s="32"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
+      <c r="AA27" s="32"/>
+      <c r="AB27" s="32"/>
+      <c r="AC27" s="32"/>
+      <c r="AD27" s="32"/>
+      <c r="AE27" s="32"/>
+      <c r="AF27" s="32"/>
+      <c r="AG27" s="32"/>
+      <c r="AH27" s="32"/>
+      <c r="AI27" s="32"/>
+      <c r="AJ27" s="32"/>
+      <c r="AK27" s="32"/>
+      <c r="AL27" s="32"/>
+      <c r="AM27" s="32"/>
+      <c r="AN27" s="32"/>
+      <c r="AO27" s="32"/>
+      <c r="AP27" s="32"/>
+    </row>
+    <row r="28" spans="1:42" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="P28" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="36"/>
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36"/>
+      <c r="AA29" s="36"/>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+    </row>
     <row r="30" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3148,11 +3457,11 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048550" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048551" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048552" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048553" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1048554" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048555" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048556" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048557" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3171,6 +3480,10 @@
     <row r="1048570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3197,67 +3510,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4267,7 +4580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4284,83 +4597,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="A1" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>86</v>
+      <c r="A2" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-04-15 21-48</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
+        <v>2020-04-22 16-03</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>